<commit_message>
feat(rule-designer-be): adding default actions and other refactorings
</commit_message>
<xml_diff>
--- a/apps/server/rule-designer-be/src/modules/seeders/seedData.xlsx
+++ b/apps/server/rule-designer-be/src/modules/seeders/seedData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="94">
   <si>
     <t>operator</t>
   </si>
@@ -259,6 +259,45 @@
   </si>
   <si>
     <t>Rule seventeen</t>
+  </si>
+  <si>
+    <t>defaultActionName</t>
+  </si>
+  <si>
+    <t>defaultActionValue</t>
+  </si>
+  <si>
+    <t>defaultIsArray</t>
+  </si>
+  <si>
+    <t>defaultActionType</t>
+  </si>
+  <si>
+    <t>possibleReasons</t>
+  </si>
+  <si>
+    <t>Adoption of new cost-effective technologies or materials that impact the quotation process.</t>
+  </si>
+  <si>
+    <t>Changes in market dynamics affecting supplier pricing strategies.</t>
+  </si>
+  <si>
+    <t>Internal initiatives to streamline the procurement process for efficiency.</t>
+  </si>
+  <si>
+    <t>Emergence of more cost-effective suppliers after the initial quotation request.</t>
+  </si>
+  <si>
+    <t>Changes in project specifications or quantities requiring revised quotations.</t>
+  </si>
+  <si>
+    <t>Legal challenges or concerns regarding the RFQ process.</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>sth</t>
   </si>
 </sst>
 </file>
@@ -609,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N94"/>
+  <dimension ref="A1:S94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F16" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -627,9 +666,10 @@
     <col min="10" max="10" width="11.33203125" customWidth="1"/>
     <col min="11" max="11" width="19.44140625" customWidth="1"/>
     <col min="12" max="12" width="17.44140625" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -672,8 +712,23 @@
       <c r="N1" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -707,8 +762,20 @@
       <c r="N2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P2" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q2" t="b">
+        <v>1</v>
+      </c>
+      <c r="S2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -730,8 +797,20 @@
       <c r="H3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1</v>
+      </c>
+      <c r="S3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -753,12 +832,15 @@
       <c r="H4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="S4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -786,14 +868,11 @@
       <c r="I6">
         <v>2</v>
       </c>
-      <c r="J6" t="s">
-        <v>52</v>
-      </c>
-      <c r="N6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="S6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -815,8 +894,11 @@
       <c r="H7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="S7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -838,12 +920,15 @@
       <c r="H8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="S8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -871,14 +956,8 @@
       <c r="I10">
         <v>3</v>
       </c>
-      <c r="J10" t="s">
-        <v>52</v>
-      </c>
-      <c r="N10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -901,7 +980,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -924,11 +1003,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
@@ -962,8 +1041,17 @@
       <c r="N14" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O14" t="s">
+        <v>5</v>
+      </c>
+      <c r="P14" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
@@ -986,7 +1074,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -1009,11 +1097,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
@@ -1041,14 +1129,8 @@
       <c r="I18">
         <v>2</v>
       </c>
-      <c r="J18" t="s">
-        <v>52</v>
-      </c>
-      <c r="N18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
@@ -1071,7 +1153,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
@@ -1094,11 +1176,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -1126,14 +1208,8 @@
       <c r="I22">
         <v>3</v>
       </c>
-      <c r="J22" t="s">
-        <v>52</v>
-      </c>
-      <c r="N22" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
@@ -1156,7 +1232,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -1179,11 +1255,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
@@ -1211,14 +1287,8 @@
       <c r="I26">
         <v>4</v>
       </c>
-      <c r="J26" t="s">
-        <v>52</v>
-      </c>
-      <c r="N26" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
@@ -1241,7 +1311,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
@@ -1264,11 +1334,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>37</v>
       </c>
@@ -1302,8 +1372,17 @@
       <c r="N30" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O30" t="s">
+        <v>5</v>
+      </c>
+      <c r="P30" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
@@ -1326,7 +1405,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
@@ -1349,11 +1428,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
@@ -1381,14 +1460,8 @@
       <c r="I34">
         <v>2</v>
       </c>
-      <c r="J34" t="s">
-        <v>52</v>
-      </c>
-      <c r="N34" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>37</v>
       </c>
@@ -1411,7 +1484,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>37</v>
       </c>
@@ -1434,11 +1507,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
@@ -1466,14 +1539,8 @@
       <c r="I38">
         <v>3</v>
       </c>
-      <c r="J38" t="s">
-        <v>52</v>
-      </c>
-      <c r="N38" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
@@ -1496,7 +1563,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>37</v>
       </c>
@@ -1519,11 +1586,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
     </row>
-    <row r="42" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>59</v>
       </c>
@@ -1557,8 +1624,17 @@
       <c r="N42" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O42" t="s">
+        <v>5</v>
+      </c>
+      <c r="P42" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>59</v>
       </c>
@@ -1581,7 +1657,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>59</v>
       </c>
@@ -1604,11 +1680,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
     </row>
-    <row r="46" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>42</v>
       </c>
@@ -1642,8 +1718,17 @@
       <c r="N46" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O46" t="s">
+        <v>5</v>
+      </c>
+      <c r="P46" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>42</v>
       </c>
@@ -1666,7 +1751,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>42</v>
       </c>
@@ -1689,11 +1774,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>56</v>
       </c>
@@ -1727,8 +1812,17 @@
       <c r="N50" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O50" t="s">
+        <v>5</v>
+      </c>
+      <c r="P50" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>56</v>
       </c>
@@ -1751,7 +1845,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>56</v>
       </c>
@@ -1774,11 +1868,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>57</v>
       </c>
@@ -1812,8 +1906,17 @@
       <c r="N54" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O54" t="s">
+        <v>5</v>
+      </c>
+      <c r="P54" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>57</v>
       </c>
@@ -1836,7 +1939,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>57</v>
       </c>
@@ -1859,11 +1962,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
     </row>
-    <row r="58" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>47</v>
       </c>
@@ -1897,8 +2000,17 @@
       <c r="N58" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O58" t="s">
+        <v>5</v>
+      </c>
+      <c r="P58" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>47</v>
       </c>
@@ -1921,7 +2033,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>47</v>
       </c>
@@ -1944,11 +2056,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>49</v>
       </c>
@@ -1982,8 +2094,17 @@
       <c r="N62" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O62" t="s">
+        <v>5</v>
+      </c>
+      <c r="P62" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>49</v>
       </c>
@@ -2006,7 +2127,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>49</v>
       </c>
@@ -2029,11 +2150,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>50</v>
       </c>
@@ -2067,8 +2188,17 @@
       <c r="N66" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O66" t="s">
+        <v>5</v>
+      </c>
+      <c r="P66" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q66" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>50</v>
       </c>
@@ -2091,7 +2221,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>50</v>
       </c>
@@ -2114,11 +2244,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>50</v>
       </c>
@@ -2146,14 +2276,8 @@
       <c r="I70">
         <v>2</v>
       </c>
-      <c r="J70" t="s">
-        <v>52</v>
-      </c>
-      <c r="N70" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>50</v>
       </c>
@@ -2176,7 +2300,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>50</v>
       </c>
@@ -2199,11 +2323,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>51</v>
       </c>
@@ -2237,8 +2361,17 @@
       <c r="N74" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O74" t="s">
+        <v>5</v>
+      </c>
+      <c r="P74" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q74" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>51</v>
       </c>
@@ -2261,7 +2394,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>51</v>
       </c>
@@ -2284,10 +2417,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>51</v>
       </c>
@@ -2315,14 +2448,8 @@
       <c r="I78">
         <v>2</v>
       </c>
-      <c r="J78" t="s">
-        <v>52</v>
-      </c>
-      <c r="N78" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>51</v>
       </c>
@@ -2345,7 +2472,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>51</v>
       </c>
@@ -2368,11 +2495,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>51</v>
       </c>
@@ -2400,14 +2527,8 @@
       <c r="I82">
         <v>3</v>
       </c>
-      <c r="J82" t="s">
-        <v>52</v>
-      </c>
-      <c r="N82" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>51</v>
       </c>
@@ -2430,7 +2551,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>51</v>
       </c>
@@ -2453,11 +2574,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
     </row>
-    <row r="86" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>61</v>
       </c>
@@ -2491,8 +2612,17 @@
       <c r="N86" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="87" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O86" t="s">
+        <v>5</v>
+      </c>
+      <c r="P86" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q86" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>61</v>
       </c>
@@ -2527,11 +2657,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1"/>
       <c r="E88" s="3"/>
     </row>
-    <row r="89" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>62</v>
       </c>
@@ -2565,8 +2695,17 @@
       <c r="N89" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O89" t="s">
+        <v>5</v>
+      </c>
+      <c r="P89" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q89" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>62</v>
       </c>
@@ -2601,7 +2740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>62</v>
       </c>
@@ -2624,7 +2763,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>62</v>
       </c>
@@ -2647,7 +2786,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>62</v>
       </c>
@@ -2670,7 +2809,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>62</v>
       </c>

</xml_diff>